<commit_message>
Update new data quiz & redesign UI
</commit_message>
<xml_diff>
--- a/Source.xlsx
+++ b/Source.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dangd\Desktop\QuizeGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QuizGame-Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEF791C-7CB6-4E10-AB6C-F8FC127DE237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F378EF72-6F6A-482E-9311-E179C0AF129E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{0194394E-8583-4E7D-ADEA-E5B20066F266}"/>
+    <workbookView xWindow="15564" yWindow="0" windowWidth="15252" windowHeight="16656" activeTab="1" xr2:uid="{0194394E-8583-4E7D-ADEA-E5B20066F266}"/>
   </bookViews>
   <sheets>
     <sheet name="Part-1" sheetId="1" r:id="rId1"/>
@@ -1111,17 +1111,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1459,7 +1459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F906B7B-1D5C-4591-98EB-D844B30F81D2}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1644,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8739D4D0-873A-4455-A7E8-DCB87D10EB3C}">
   <dimension ref="A1:C137"/>
   <sheetViews>
-    <sheetView topLeftCell="A123" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1675,10 +1675,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" s="14" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="25">
+      <c r="A3" s="24">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="26" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -1686,38 +1686,38 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="24"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="14" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="24"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="24"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="24"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="A8" s="24">
         <v>2</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="26" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -1725,38 +1725,38 @@
       </c>
     </row>
     <row r="9" spans="1:3" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="24"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="24"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="24"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="14" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="25">
+      <c r="A13" s="24">
         <v>3</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="15" t="s">
@@ -1764,38 +1764,38 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="24"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="15" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="24"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="15" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="24"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="25">
+      <c r="A18" s="24">
         <v>4</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="26" t="s">
         <v>41</v>
       </c>
       <c r="C18" s="15" t="s">
@@ -1803,38 +1803,38 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="24"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="15" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="24"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="15" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="24"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="15" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="24"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="25">
+      <c r="A23" s="24">
         <v>5</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="26" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="15" t="s">
@@ -1842,38 +1842,38 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="24"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="24"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="15" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
-      <c r="B26" s="24"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="15" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
-      <c r="B27" s="24"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25">
+      <c r="A28" s="24">
         <v>6</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="27" t="s">
         <v>53</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1881,38 +1881,38 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="26"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="26"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="26"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="27"/>
       <c r="C31" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="26"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A33" s="25">
+      <c r="A33" s="24">
         <v>7</v>
       </c>
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C33" s="15" t="s">
@@ -1920,38 +1920,38 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="24"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="24"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="24"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="24"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A38" s="25">
+      <c r="A38" s="24">
         <v>8</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="26" t="s">
         <v>65</v>
       </c>
       <c r="C38" s="15" t="s">
@@ -1959,38 +1959,38 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="24"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="24"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="26"/>
       <c r="C40" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="24"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
-      <c r="B42" s="24"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="26"/>
       <c r="C42" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A43" s="25">
+      <c r="A43" s="24">
         <v>9</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="26" t="s">
         <v>71</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -1998,38 +1998,38 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
-      <c r="B44" s="24"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
-      <c r="B45" s="24"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
-      <c r="B46" s="24"/>
+      <c r="A46" s="24"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="16" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="25"/>
-      <c r="B47" s="24"/>
+      <c r="A47" s="24"/>
+      <c r="B47" s="26"/>
       <c r="C47" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A48" s="25">
+      <c r="A48" s="24">
         <v>10</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B48" s="26" t="s">
         <v>77</v>
       </c>
       <c r="C48" s="17" t="s">
@@ -2037,38 +2037,38 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
-      <c r="B49" s="24"/>
+      <c r="A49" s="24"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
-      <c r="B50" s="24"/>
+      <c r="A50" s="24"/>
+      <c r="B50" s="26"/>
       <c r="C50" s="16" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
-      <c r="B51" s="24"/>
+      <c r="A51" s="24"/>
+      <c r="B51" s="26"/>
       <c r="C51" s="16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
-      <c r="B52" s="24"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="26"/>
       <c r="C52" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A53" s="25">
+      <c r="A53" s="24">
         <v>11</v>
       </c>
-      <c r="B53" s="24" t="s">
+      <c r="B53" s="26" t="s">
         <v>83</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2076,38 +2076,38 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="25"/>
-      <c r="B54" s="24"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="26"/>
       <c r="C54" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
-      <c r="B55" s="24"/>
+      <c r="A55" s="24"/>
+      <c r="B55" s="26"/>
       <c r="C55" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A56" s="25"/>
-      <c r="B56" s="24"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="26"/>
       <c r="C56" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
-      <c r="B57" s="24"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="26"/>
       <c r="C57" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="25">
+      <c r="A58" s="24">
         <v>12</v>
       </c>
-      <c r="B58" s="24" t="s">
+      <c r="B58" s="26" t="s">
         <v>89</v>
       </c>
       <c r="C58" s="17" t="s">
@@ -2115,38 +2115,38 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="25"/>
-      <c r="B59" s="24"/>
+      <c r="A59" s="24"/>
+      <c r="B59" s="26"/>
       <c r="C59" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="25"/>
-      <c r="B60" s="24"/>
+      <c r="A60" s="24"/>
+      <c r="B60" s="26"/>
       <c r="C60" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="25"/>
-      <c r="B61" s="24"/>
+      <c r="A61" s="24"/>
+      <c r="B61" s="26"/>
       <c r="C61" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="25"/>
-      <c r="B62" s="24"/>
+      <c r="A62" s="24"/>
+      <c r="B62" s="26"/>
       <c r="C62" s="16" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="25">
+      <c r="A63" s="24">
         <v>13</v>
       </c>
-      <c r="B63" s="24" t="s">
+      <c r="B63" s="26" t="s">
         <v>95</v>
       </c>
       <c r="C63" s="3" t="s">
@@ -2154,38 +2154,38 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
-      <c r="B64" s="24"/>
+      <c r="A64" s="24"/>
+      <c r="B64" s="26"/>
       <c r="C64" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A65" s="25"/>
-      <c r="B65" s="24"/>
+      <c r="A65" s="24"/>
+      <c r="B65" s="26"/>
       <c r="C65" s="16" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A66" s="25"/>
-      <c r="B66" s="24"/>
+      <c r="A66" s="24"/>
+      <c r="B66" s="26"/>
       <c r="C66" s="16" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="25"/>
-      <c r="B67" s="24"/>
+      <c r="A67" s="24"/>
+      <c r="B67" s="26"/>
       <c r="C67" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A68" s="25">
+      <c r="A68" s="24">
         <v>14</v>
       </c>
-      <c r="B68" s="24" t="s">
+      <c r="B68" s="26" t="s">
         <v>101</v>
       </c>
       <c r="C68" s="3" t="s">
@@ -2193,38 +2193,38 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A69" s="25"/>
-      <c r="B69" s="24"/>
+      <c r="A69" s="24"/>
+      <c r="B69" s="26"/>
       <c r="C69" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="25"/>
-      <c r="B70" s="24"/>
+      <c r="A70" s="24"/>
+      <c r="B70" s="26"/>
       <c r="C70" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="25"/>
-      <c r="B71" s="24"/>
+      <c r="A71" s="24"/>
+      <c r="B71" s="26"/>
       <c r="C71" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A72" s="25"/>
-      <c r="B72" s="24"/>
+      <c r="A72" s="24"/>
+      <c r="B72" s="26"/>
       <c r="C72" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="25">
+      <c r="A73" s="24">
         <v>15</v>
       </c>
-      <c r="B73" s="24" t="s">
+      <c r="B73" s="26" t="s">
         <v>107</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -2232,38 +2232,38 @@
       </c>
     </row>
     <row r="74" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A74" s="25"/>
-      <c r="B74" s="24"/>
+      <c r="A74" s="24"/>
+      <c r="B74" s="26"/>
       <c r="C74" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A75" s="25"/>
-      <c r="B75" s="24"/>
+      <c r="A75" s="24"/>
+      <c r="B75" s="26"/>
       <c r="C75" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="25"/>
-      <c r="B76" s="24"/>
+      <c r="A76" s="24"/>
+      <c r="B76" s="26"/>
       <c r="C76" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A77" s="25"/>
-      <c r="B77" s="24"/>
+      <c r="A77" s="24"/>
+      <c r="B77" s="26"/>
       <c r="C77" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="25">
+      <c r="A78" s="24">
         <v>16</v>
       </c>
-      <c r="B78" s="27" t="s">
+      <c r="B78" s="25" t="s">
         <v>113</v>
       </c>
       <c r="C78" s="3" t="s">
@@ -2271,38 +2271,38 @@
       </c>
     </row>
     <row r="79" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A79" s="25"/>
-      <c r="B79" s="27"/>
+      <c r="A79" s="24"/>
+      <c r="B79" s="25"/>
       <c r="C79" s="3" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A80" s="25"/>
-      <c r="B80" s="27"/>
+      <c r="A80" s="24"/>
+      <c r="B80" s="25"/>
       <c r="C80" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="25"/>
-      <c r="B81" s="27"/>
+      <c r="A81" s="24"/>
+      <c r="B81" s="25"/>
       <c r="C81" s="3" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="25"/>
-      <c r="B82" s="27"/>
+      <c r="A82" s="24"/>
+      <c r="B82" s="25"/>
       <c r="C82" s="3" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="25">
+      <c r="A83" s="24">
         <v>17</v>
       </c>
-      <c r="B83" s="27" t="s">
+      <c r="B83" s="25" t="s">
         <v>119</v>
       </c>
       <c r="C83" s="3" t="s">
@@ -2310,38 +2310,38 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="25"/>
-      <c r="B84" s="27"/>
+      <c r="A84" s="24"/>
+      <c r="B84" s="25"/>
       <c r="C84" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="25"/>
-      <c r="B85" s="27"/>
+      <c r="A85" s="24"/>
+      <c r="B85" s="25"/>
       <c r="C85" s="3" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="25"/>
-      <c r="B86" s="27"/>
+      <c r="A86" s="24"/>
+      <c r="B86" s="25"/>
       <c r="C86" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="25"/>
-      <c r="B87" s="27"/>
+      <c r="A87" s="24"/>
+      <c r="B87" s="25"/>
       <c r="C87" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A88" s="25">
+      <c r="A88" s="24">
         <v>18</v>
       </c>
-      <c r="B88" s="24" t="s">
+      <c r="B88" s="26" t="s">
         <v>125</v>
       </c>
       <c r="C88" s="3" t="s">
@@ -2349,38 +2349,38 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="25"/>
-      <c r="B89" s="24"/>
+      <c r="A89" s="24"/>
+      <c r="B89" s="26"/>
       <c r="C89" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="25"/>
-      <c r="B90" s="24"/>
+      <c r="A90" s="24"/>
+      <c r="B90" s="26"/>
       <c r="C90" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="25"/>
-      <c r="B91" s="24"/>
+      <c r="A91" s="24"/>
+      <c r="B91" s="26"/>
       <c r="C91" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A92" s="25"/>
-      <c r="B92" s="24"/>
+      <c r="A92" s="24"/>
+      <c r="B92" s="26"/>
       <c r="C92" s="3" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A93" s="25">
+      <c r="A93" s="24">
         <v>19</v>
       </c>
-      <c r="B93" s="24" t="s">
+      <c r="B93" s="26" t="s">
         <v>131</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -2388,38 +2388,38 @@
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="25"/>
-      <c r="B94" s="24"/>
+      <c r="A94" s="24"/>
+      <c r="B94" s="26"/>
       <c r="C94" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A95" s="25"/>
-      <c r="B95" s="24"/>
+      <c r="A95" s="24"/>
+      <c r="B95" s="26"/>
       <c r="C95" s="3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A96" s="25"/>
-      <c r="B96" s="24"/>
+      <c r="A96" s="24"/>
+      <c r="B96" s="26"/>
       <c r="C96" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A97" s="25"/>
-      <c r="B97" s="24"/>
+      <c r="A97" s="24"/>
+      <c r="B97" s="26"/>
       <c r="C97" s="3" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="25">
+      <c r="A98" s="24">
         <v>20</v>
       </c>
-      <c r="B98" s="27" t="s">
+      <c r="B98" s="25" t="s">
         <v>137</v>
       </c>
       <c r="C98" s="3" t="s">
@@ -2427,38 +2427,38 @@
       </c>
     </row>
     <row r="99" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A99" s="25"/>
-      <c r="B99" s="27"/>
+      <c r="A99" s="24"/>
+      <c r="B99" s="25"/>
       <c r="C99" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A100" s="25"/>
-      <c r="B100" s="27"/>
+      <c r="A100" s="24"/>
+      <c r="B100" s="25"/>
       <c r="C100" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A101" s="25"/>
-      <c r="B101" s="27"/>
+      <c r="A101" s="24"/>
+      <c r="B101" s="25"/>
       <c r="C101" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="25"/>
-      <c r="B102" s="27"/>
+      <c r="A102" s="24"/>
+      <c r="B102" s="25"/>
       <c r="C102" s="3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="25">
+      <c r="A103" s="24">
         <v>21</v>
       </c>
-      <c r="B103" s="24" t="s">
+      <c r="B103" s="26" t="s">
         <v>143</v>
       </c>
       <c r="C103" s="3" t="s">
@@ -2466,38 +2466,38 @@
       </c>
     </row>
     <row r="104" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A104" s="25"/>
-      <c r="B104" s="24"/>
+      <c r="A104" s="24"/>
+      <c r="B104" s="26"/>
       <c r="C104" s="3" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A105" s="25"/>
-      <c r="B105" s="24"/>
+      <c r="A105" s="24"/>
+      <c r="B105" s="26"/>
       <c r="C105" s="3" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A106" s="25"/>
-      <c r="B106" s="24"/>
+      <c r="A106" s="24"/>
+      <c r="B106" s="26"/>
       <c r="C106" s="3" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A107" s="25"/>
-      <c r="B107" s="24"/>
+      <c r="A107" s="24"/>
+      <c r="B107" s="26"/>
       <c r="C107" s="3" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A108" s="25">
+      <c r="A108" s="24">
         <v>22</v>
       </c>
-      <c r="B108" s="24" t="s">
+      <c r="B108" s="26" t="s">
         <v>149</v>
       </c>
       <c r="C108" s="3" t="s">
@@ -2505,38 +2505,38 @@
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="25"/>
-      <c r="B109" s="24"/>
+      <c r="A109" s="24"/>
+      <c r="B109" s="26"/>
       <c r="C109" s="3" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A110" s="25"/>
-      <c r="B110" s="24"/>
+      <c r="A110" s="24"/>
+      <c r="B110" s="26"/>
       <c r="C110" s="3" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A111" s="25"/>
-      <c r="B111" s="24"/>
+      <c r="A111" s="24"/>
+      <c r="B111" s="26"/>
       <c r="C111" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="25"/>
-      <c r="B112" s="24"/>
+      <c r="A112" s="24"/>
+      <c r="B112" s="26"/>
       <c r="C112" s="3" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A113" s="25">
+      <c r="A113" s="24">
         <v>23</v>
       </c>
-      <c r="B113" s="24" t="s">
+      <c r="B113" s="26" t="s">
         <v>150</v>
       </c>
       <c r="C113" s="3" t="s">
@@ -2544,38 +2544,38 @@
       </c>
     </row>
     <row r="114" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A114" s="25"/>
-      <c r="B114" s="24"/>
+      <c r="A114" s="24"/>
+      <c r="B114" s="26"/>
       <c r="C114" s="3" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A115" s="25"/>
-      <c r="B115" s="24"/>
+      <c r="A115" s="24"/>
+      <c r="B115" s="26"/>
       <c r="C115" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A116" s="25"/>
-      <c r="B116" s="24"/>
+      <c r="A116" s="24"/>
+      <c r="B116" s="26"/>
       <c r="C116" s="3" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A117" s="25"/>
-      <c r="B117" s="24"/>
+      <c r="A117" s="24"/>
+      <c r="B117" s="26"/>
       <c r="C117" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A118" s="25">
+      <c r="A118" s="24">
         <v>24</v>
       </c>
-      <c r="B118" s="27" t="s">
+      <c r="B118" s="25" t="s">
         <v>151</v>
       </c>
       <c r="C118" s="21" t="s">
@@ -2583,38 +2583,38 @@
       </c>
     </row>
     <row r="119" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A119" s="25"/>
-      <c r="B119" s="27"/>
+      <c r="A119" s="24"/>
+      <c r="B119" s="25"/>
       <c r="C119" s="21" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A120" s="25"/>
-      <c r="B120" s="27"/>
+      <c r="A120" s="24"/>
+      <c r="B120" s="25"/>
       <c r="C120" s="21" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="25"/>
-      <c r="B121" s="27"/>
+      <c r="A121" s="24"/>
+      <c r="B121" s="25"/>
       <c r="C121" s="21" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="25"/>
-      <c r="B122" s="27"/>
+      <c r="A122" s="24"/>
+      <c r="B122" s="25"/>
       <c r="C122" s="21" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A123" s="25">
+      <c r="A123" s="24">
         <v>25</v>
       </c>
-      <c r="B123" s="27" t="s">
+      <c r="B123" s="25" t="s">
         <v>152</v>
       </c>
       <c r="C123" s="22" t="s">
@@ -2622,38 +2622,38 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A124" s="25"/>
-      <c r="B124" s="27"/>
+      <c r="A124" s="24"/>
+      <c r="B124" s="25"/>
       <c r="C124" s="22" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A125" s="25"/>
-      <c r="B125" s="27"/>
+      <c r="A125" s="24"/>
+      <c r="B125" s="25"/>
       <c r="C125" s="21" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A126" s="25"/>
-      <c r="B126" s="27"/>
+      <c r="A126" s="24"/>
+      <c r="B126" s="25"/>
       <c r="C126" s="22" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="25"/>
-      <c r="B127" s="27"/>
+      <c r="A127" s="24"/>
+      <c r="B127" s="25"/>
       <c r="C127" s="22" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="25">
+      <c r="A128" s="24">
         <v>26</v>
       </c>
-      <c r="B128" s="27" t="s">
+      <c r="B128" s="25" t="s">
         <v>153</v>
       </c>
       <c r="C128" s="15" t="s">
@@ -2661,38 +2661,38 @@
       </c>
     </row>
     <row r="129" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A129" s="25"/>
-      <c r="B129" s="27"/>
+      <c r="A129" s="24"/>
+      <c r="B129" s="25"/>
       <c r="C129" s="15" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A130" s="25"/>
-      <c r="B130" s="27"/>
+      <c r="A130" s="24"/>
+      <c r="B130" s="25"/>
       <c r="C130" s="15" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A131" s="25"/>
-      <c r="B131" s="27"/>
+      <c r="A131" s="24"/>
+      <c r="B131" s="25"/>
       <c r="C131" s="15" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A132" s="25"/>
-      <c r="B132" s="27"/>
+      <c r="A132" s="24"/>
+      <c r="B132" s="25"/>
       <c r="C132" s="3" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A133" s="25">
+      <c r="A133" s="24">
         <v>27</v>
       </c>
-      <c r="B133" s="27" t="s">
+      <c r="B133" s="25" t="s">
         <v>159</v>
       </c>
       <c r="C133" s="15" t="s">
@@ -2700,43 +2700,65 @@
       </c>
     </row>
     <row r="134" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A134" s="25"/>
-      <c r="B134" s="27"/>
+      <c r="A134" s="24"/>
+      <c r="B134" s="25"/>
       <c r="C134" s="15" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A135" s="25"/>
-      <c r="B135" s="27"/>
+      <c r="A135" s="24"/>
+      <c r="B135" s="25"/>
       <c r="C135" s="15" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A136" s="25"/>
-      <c r="B136" s="27"/>
+      <c r="A136" s="24"/>
+      <c r="B136" s="25"/>
       <c r="C136" s="15" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="25"/>
-      <c r="B137" s="27"/>
+      <c r="A137" s="24"/>
+      <c r="B137" s="25"/>
       <c r="C137" s="3" t="s">
         <v>164</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A133:A137"/>
-    <mergeCell ref="B133:B137"/>
-    <mergeCell ref="A118:A122"/>
-    <mergeCell ref="B118:B122"/>
-    <mergeCell ref="A123:A127"/>
-    <mergeCell ref="B123:B127"/>
-    <mergeCell ref="A128:A132"/>
-    <mergeCell ref="B128:B132"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="B33:B37"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B108:B112"/>
+    <mergeCell ref="A108:A112"/>
+    <mergeCell ref="A103:A107"/>
+    <mergeCell ref="B103:B107"/>
+    <mergeCell ref="A98:A102"/>
+    <mergeCell ref="B98:B102"/>
+    <mergeCell ref="A63:A67"/>
+    <mergeCell ref="B63:B67"/>
+    <mergeCell ref="B93:B97"/>
+    <mergeCell ref="A93:A97"/>
+    <mergeCell ref="A88:A92"/>
+    <mergeCell ref="B88:B92"/>
     <mergeCell ref="A33:A37"/>
     <mergeCell ref="A113:A117"/>
     <mergeCell ref="B113:B117"/>
@@ -2753,36 +2775,14 @@
     <mergeCell ref="A78:A82"/>
     <mergeCell ref="A83:A87"/>
     <mergeCell ref="A43:A47"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="B108:B112"/>
-    <mergeCell ref="A108:A112"/>
-    <mergeCell ref="A103:A107"/>
-    <mergeCell ref="B103:B107"/>
-    <mergeCell ref="A98:A102"/>
-    <mergeCell ref="B98:B102"/>
-    <mergeCell ref="A63:A67"/>
-    <mergeCell ref="B63:B67"/>
-    <mergeCell ref="B93:B97"/>
-    <mergeCell ref="A93:A97"/>
-    <mergeCell ref="A88:A92"/>
-    <mergeCell ref="B88:B92"/>
-    <mergeCell ref="B83:B87"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A133:A137"/>
+    <mergeCell ref="B133:B137"/>
+    <mergeCell ref="A118:A122"/>
+    <mergeCell ref="B118:B122"/>
+    <mergeCell ref="A123:A127"/>
+    <mergeCell ref="B123:B127"/>
+    <mergeCell ref="A128:A132"/>
+    <mergeCell ref="B128:B132"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>